<commit_message>
fix: Fixed Sigungu Enum #21
</commit_message>
<xml_diff>
--- a/src/main/resources/data/excel/test_coordinates_excel.xlsx
+++ b/src/main/resources/data/excel/test_coordinates_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\이승영\Desktop\융복합_국내+지역별+관광명소(2023)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9615B1-DC34-48A6-BE91-0B9FCF10AB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD809D8-C527-4AA4-A47A-FE5F6595385E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="468" yWindow="240" windowWidth="16656" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5412" yWindow="516" windowWidth="17328" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="146">
   <si>
     <t>CTPR_NM</t>
   </si>
@@ -89,6 +89,381 @@
   <si>
     <t>LC_LO</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>강서구</t>
+  </si>
+  <si>
+    <t>마곡동</t>
+  </si>
+  <si>
+    <t>뉴코리아여행사</t>
+  </si>
+  <si>
+    <t>반도에어에이젠시</t>
+  </si>
+  <si>
+    <t>펜션다나와</t>
+  </si>
+  <si>
+    <t>SJTRAVELCOLTD</t>
+  </si>
+  <si>
+    <t>브엘로항공</t>
+  </si>
+  <si>
+    <t>구로구</t>
+  </si>
+  <si>
+    <t>가리봉동</t>
+  </si>
+  <si>
+    <t>천안문여행사행정사</t>
+  </si>
+  <si>
+    <t>JC북경취업행정여행사</t>
+  </si>
+  <si>
+    <t>구로동</t>
+  </si>
+  <si>
+    <t>투어컴</t>
+  </si>
+  <si>
+    <t>선우여행사</t>
+  </si>
+  <si>
+    <t>깔깔거리</t>
+  </si>
+  <si>
+    <t>먹거리/패션거리</t>
+  </si>
+  <si>
+    <t>천우여행사</t>
+  </si>
+  <si>
+    <t>광주광역시</t>
+  </si>
+  <si>
+    <t>북구</t>
+  </si>
+  <si>
+    <t>신안동</t>
+  </si>
+  <si>
+    <t>토마토여행사</t>
+  </si>
+  <si>
+    <t>충효동</t>
+  </si>
+  <si>
+    <t>무등산평촌명품마을</t>
+  </si>
+  <si>
+    <t>월출동</t>
+  </si>
+  <si>
+    <t>광주시민의숲야영장</t>
+  </si>
+  <si>
+    <t>야영장</t>
+  </si>
+  <si>
+    <t>청풍동</t>
+  </si>
+  <si>
+    <t>청풍지구탐방지원센터</t>
+  </si>
+  <si>
+    <t>관광안내소/매표소</t>
+  </si>
+  <si>
+    <t>임동</t>
+  </si>
+  <si>
+    <t>광주자동차의거리</t>
+  </si>
+  <si>
+    <t>인천광역시</t>
+  </si>
+  <si>
+    <t>남동구</t>
+  </si>
+  <si>
+    <t>간석동</t>
+  </si>
+  <si>
+    <t>그랜드항공여행사</t>
+  </si>
+  <si>
+    <t>삼화여행사</t>
+  </si>
+  <si>
+    <t>하늘여행</t>
+  </si>
+  <si>
+    <t>화인투어</t>
+  </si>
+  <si>
+    <t>구월동</t>
+  </si>
+  <si>
+    <t>미래교육여행투어</t>
+  </si>
+  <si>
+    <t>충청북도</t>
+  </si>
+  <si>
+    <t>단양군</t>
+  </si>
+  <si>
+    <t>단양읍</t>
+  </si>
+  <si>
+    <t>천동리</t>
+  </si>
+  <si>
+    <t>천동제1오토캠핑장</t>
+  </si>
+  <si>
+    <t>캠핑장</t>
+  </si>
+  <si>
+    <t>노동리</t>
+  </si>
+  <si>
+    <t>노동동굴</t>
+  </si>
+  <si>
+    <t>유명사적/유적지</t>
+  </si>
+  <si>
+    <t>대강면</t>
+  </si>
+  <si>
+    <t>사인암리</t>
+  </si>
+  <si>
+    <t>수운정</t>
+  </si>
+  <si>
+    <t>천동동굴</t>
+  </si>
+  <si>
+    <t>단성면</t>
+  </si>
+  <si>
+    <t>하방리</t>
+  </si>
+  <si>
+    <t>단양적성비</t>
+  </si>
+  <si>
+    <t>경상북도</t>
+  </si>
+  <si>
+    <t>울릉군</t>
+  </si>
+  <si>
+    <t>울릉읍</t>
+  </si>
+  <si>
+    <t>도동리</t>
+  </si>
+  <si>
+    <t>울릉도여행2</t>
+  </si>
+  <si>
+    <t>까치투어</t>
+  </si>
+  <si>
+    <t>섬목여행사</t>
+  </si>
+  <si>
+    <t>경상남도</t>
+  </si>
+  <si>
+    <t>거창군</t>
+  </si>
+  <si>
+    <t>가조면</t>
+  </si>
+  <si>
+    <t>수월리</t>
+  </si>
+  <si>
+    <t>우두산출렁다리</t>
+  </si>
+  <si>
+    <t>고제면</t>
+  </si>
+  <si>
+    <t>개명리</t>
+  </si>
+  <si>
+    <t>빼재산림레포츠파크</t>
+  </si>
+  <si>
+    <t>테마공원/대형놀이공원</t>
+  </si>
+  <si>
+    <t>웅양면</t>
+  </si>
+  <si>
+    <t>노현리</t>
+  </si>
+  <si>
+    <t>곰내미체험마을</t>
+  </si>
+  <si>
+    <t>팜스테이</t>
+  </si>
+  <si>
+    <t>위천면</t>
+  </si>
+  <si>
+    <t>장기리</t>
+  </si>
+  <si>
+    <t>거창서핑파크글램핑</t>
+  </si>
+  <si>
+    <t>거창읍</t>
+  </si>
+  <si>
+    <t>상림리</t>
+  </si>
+  <si>
+    <t>하나투어</t>
+  </si>
+  <si>
+    <t>거창항노화힐링랜드</t>
+  </si>
+  <si>
+    <t>대평리</t>
+  </si>
+  <si>
+    <t>거창백두관광</t>
+  </si>
+  <si>
+    <t>김천리</t>
+  </si>
+  <si>
+    <t>계명여행사</t>
+  </si>
+  <si>
+    <t>강원도</t>
+  </si>
+  <si>
+    <t>양양군</t>
+  </si>
+  <si>
+    <t>현남면</t>
+  </si>
+  <si>
+    <t>원포리</t>
+  </si>
+  <si>
+    <t>원포해수욕장야영장</t>
+  </si>
+  <si>
+    <t>서면</t>
+  </si>
+  <si>
+    <t>오색리</t>
+  </si>
+  <si>
+    <t>흘림골탐방지원센터</t>
+  </si>
+  <si>
+    <t>북분리</t>
+  </si>
+  <si>
+    <t>로마드협동조합</t>
+  </si>
+  <si>
+    <t>전라북도</t>
+  </si>
+  <si>
+    <t>전주시 완산구</t>
+  </si>
+  <si>
+    <t>서신동</t>
+  </si>
+  <si>
+    <t>세계로여행사</t>
+  </si>
+  <si>
+    <t>서노송동</t>
+  </si>
+  <si>
+    <t>전북관광안내소</t>
+  </si>
+  <si>
+    <t>상림동</t>
+  </si>
+  <si>
+    <t>전주영화종합촬영소</t>
+  </si>
+  <si>
+    <t>드라마/영화촬영지</t>
+  </si>
+  <si>
+    <t>중화산동2가</t>
+  </si>
+  <si>
+    <t>중화산가구거리</t>
+  </si>
+  <si>
+    <t>제주특별자치도</t>
+  </si>
+  <si>
+    <t>제주시</t>
+  </si>
+  <si>
+    <t>노형동</t>
+  </si>
+  <si>
+    <t>썬앤문투어</t>
+  </si>
+  <si>
+    <t>삼도일동</t>
+  </si>
+  <si>
+    <t>뭉치</t>
+  </si>
+  <si>
+    <t>이도이동</t>
+  </si>
+  <si>
+    <t>제주가자</t>
+  </si>
+  <si>
+    <t>제주골프투어</t>
+  </si>
+  <si>
+    <t>대흥국제여행사</t>
+  </si>
+  <si>
+    <t>한림읍</t>
+  </si>
+  <si>
+    <t>귀덕리</t>
+  </si>
+  <si>
+    <t>정원스카이</t>
+  </si>
+  <si>
+    <t>아라일동</t>
+  </si>
+  <si>
+    <t>제이제이글로벌</t>
+  </si>
+  <si>
+    <t>연동</t>
+  </si>
+  <si>
+    <t>에이오티브이</t>
   </si>
 </sst>
 </file>
@@ -425,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -582,6 +957,1294 @@
         <v>11</v>
       </c>
     </row>
+    <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="2">
+        <v>126.8313646</v>
+      </c>
+      <c r="F7" s="2">
+        <v>37.559693809999999</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2">
+        <v>126.8262567</v>
+      </c>
+      <c r="F8" s="2">
+        <v>37.558610209999998</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="2">
+        <v>126.8274467</v>
+      </c>
+      <c r="F9" s="2">
+        <v>37.558472780000002</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="2">
+        <v>126.8242396</v>
+      </c>
+      <c r="F10" s="2">
+        <v>37.558796970000003</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="2">
+        <v>126.8242396</v>
+      </c>
+      <c r="F11" s="2">
+        <v>37.558796970000003</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="2">
+        <v>126.8872914</v>
+      </c>
+      <c r="F12" s="2">
+        <v>37.482868789999998</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="2">
+        <v>126.8862407</v>
+      </c>
+      <c r="F13" s="2">
+        <v>37.484098189999997</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="2">
+        <v>126.8750625</v>
+      </c>
+      <c r="F14" s="2">
+        <v>37.485606599999997</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="2">
+        <v>126.8848504</v>
+      </c>
+      <c r="F15" s="2">
+        <v>37.48825008</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="2">
+        <v>126.9008822</v>
+      </c>
+      <c r="F16" s="2">
+        <v>37.483956390000003</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="2">
+        <v>126.8861907</v>
+      </c>
+      <c r="F17" s="2">
+        <v>37.490914160000003</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="2">
+        <v>126.9029379</v>
+      </c>
+      <c r="F18" s="2">
+        <v>35.165219610000001</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="2">
+        <v>127.01051339999999</v>
+      </c>
+      <c r="F19" s="2">
+        <v>35.175610720000002</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="2">
+        <v>126.8688384</v>
+      </c>
+      <c r="F20" s="2">
+        <v>35.23782053</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="2">
+        <v>126.96224669999999</v>
+      </c>
+      <c r="F21" s="2">
+        <v>35.16259968</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="2">
+        <v>126.8999699</v>
+      </c>
+      <c r="F22" s="2">
+        <v>35.159557489999997</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="2">
+        <v>126.70385659999999</v>
+      </c>
+      <c r="F23" s="2">
+        <v>37.456895430000003</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="2">
+        <v>126.708539</v>
+      </c>
+      <c r="F24" s="2">
+        <v>37.462719139999997</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="2">
+        <v>126.7082996</v>
+      </c>
+      <c r="F25" s="2">
+        <v>37.468343490000002</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="2">
+        <v>126.71691319999999</v>
+      </c>
+      <c r="F26" s="2">
+        <v>37.463170179999999</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="2">
+        <v>126.7027776</v>
+      </c>
+      <c r="F27" s="2">
+        <v>37.453066790000001</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" s="2">
+        <v>128.41721319999999</v>
+      </c>
+      <c r="F28" s="2">
+        <v>36.973149579999998</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="2">
+        <v>128.38179690000001</v>
+      </c>
+      <c r="F29" s="2">
+        <v>36.952974009999998</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" s="2">
+        <v>128.3403955</v>
+      </c>
+      <c r="F30" s="2">
+        <v>36.894278980000003</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E31" s="2">
+        <v>128.4222695</v>
+      </c>
+      <c r="F31" s="2">
+        <v>36.970544080000003</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E32" s="2">
+        <v>128.3210244</v>
+      </c>
+      <c r="F32" s="2">
+        <v>36.94429238</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" s="2">
+        <v>130.90878119999999</v>
+      </c>
+      <c r="F33" s="2">
+        <v>37.492099680000003</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E34" s="2">
+        <v>130.90787169999999</v>
+      </c>
+      <c r="F34" s="2">
+        <v>37.482199260000002</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E35" s="2">
+        <v>130.90870670000001</v>
+      </c>
+      <c r="F35" s="2">
+        <v>37.492564119999997</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E36" s="2">
+        <v>128.0456092</v>
+      </c>
+      <c r="F36" s="2">
+        <v>35.738128420000002</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E37" s="2">
+        <v>127.83127690000001</v>
+      </c>
+      <c r="F37" s="2">
+        <v>35.8590917</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E38" s="2">
+        <v>127.91547869999999</v>
+      </c>
+      <c r="F38" s="2">
+        <v>35.80179854</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E39" s="2">
+        <v>127.83690729999999</v>
+      </c>
+      <c r="F39" s="2">
+        <v>35.747887390000002</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E40" s="2">
+        <v>127.9081321</v>
+      </c>
+      <c r="F40" s="2">
+        <v>35.689240720000001</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E41" s="2">
+        <v>128.04090869999999</v>
+      </c>
+      <c r="F41" s="2">
+        <v>35.736698390000001</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E42" s="2">
+        <v>127.9207523</v>
+      </c>
+      <c r="F42" s="2">
+        <v>35.686184099999998</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E43" s="2">
+        <v>127.9110766</v>
+      </c>
+      <c r="F43" s="2">
+        <v>35.675875599999998</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E44" s="2">
+        <v>128.7906725</v>
+      </c>
+      <c r="F44" s="2">
+        <v>37.932336100000001</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E45" s="2">
+        <v>128.42137149999999</v>
+      </c>
+      <c r="F45" s="2">
+        <v>38.088952990000003</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E46" s="2">
+        <v>128.74240689999999</v>
+      </c>
+      <c r="F46" s="2">
+        <v>37.98048644</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" s="2">
+        <v>127.12239719999999</v>
+      </c>
+      <c r="F47" s="2">
+        <v>35.83034086</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D48" s="1"/>
+      <c r="E48" s="2">
+        <v>127.1492794</v>
+      </c>
+      <c r="F48" s="2">
+        <v>35.8233101</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D49" s="1"/>
+      <c r="E49" s="2">
+        <v>127.07510190000001</v>
+      </c>
+      <c r="F49" s="2">
+        <v>35.814716330000003</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D50" s="1"/>
+      <c r="E50" s="2">
+        <v>127.12145270000001</v>
+      </c>
+      <c r="F50" s="2">
+        <v>35.81258716</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D51" s="1"/>
+      <c r="E51" s="2">
+        <v>126.4846084</v>
+      </c>
+      <c r="F51" s="2">
+        <v>33.488691799999998</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="2">
+        <v>126.5231656</v>
+      </c>
+      <c r="F52" s="2">
+        <v>33.499992030000001</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D53" s="1"/>
+      <c r="E53" s="2">
+        <v>126.5322551</v>
+      </c>
+      <c r="F53" s="2">
+        <v>33.496968170000002</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="2">
+        <v>126.4846084</v>
+      </c>
+      <c r="F54" s="2">
+        <v>33.488691799999998</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D55" s="1"/>
+      <c r="E55" s="2">
+        <v>126.5428515</v>
+      </c>
+      <c r="F55" s="2">
+        <v>33.501386529999998</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E56" s="2">
+        <v>126.27621120000001</v>
+      </c>
+      <c r="F56" s="2">
+        <v>33.43284259</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D57" s="1"/>
+      <c r="E57" s="2">
+        <v>126.5487505</v>
+      </c>
+      <c r="F57" s="2">
+        <v>33.465902960000001</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D58" s="1"/>
+      <c r="E58" s="2">
+        <v>126.4911132</v>
+      </c>
+      <c r="F58" s="2">
+        <v>33.488571139999998</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>